<commit_message>
Updated DMB -- Version Flow on Osprey
</commit_message>
<xml_diff>
--- a/DataManagementBoard_V3/Bill of Materials-DataManagementBoard_V3.xlsx
+++ b/DataManagementBoard_V3/Bill of Materials-DataManagementBoard_V3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2020 - 2021\Andromeda-V3.2\DataManagementBoard_V3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\randy\Documents\GitHub\Andromeda-V3.3\DataManagementBoard_V3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A06DC4A-E943-491A-9C4A-69C22D781BAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23145B5B-9360-48F9-B0C8-9E0905554FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15690" yWindow="2670" windowWidth="14400" windowHeight="7365" xr2:uid="{3D4BD06D-1139-467C-B010-4B4921899CC2}"/>
+    <workbookView xWindow="0" yWindow="372" windowWidth="21600" windowHeight="11328" xr2:uid="{3D4BD06D-1139-467C-B010-4B4921899CC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-DataManagemen" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
   <si>
     <t>Comment</t>
   </si>
@@ -292,6 +292,18 @@
   </si>
   <si>
     <t>C7, C19</t>
+  </si>
+  <si>
+    <t>BACKORDER</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Backorder</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -321,7 +333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -344,11 +356,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -358,6 +379,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -677,18 +704,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="18.81640625" customWidth="1"/>
+    <col min="1" max="6" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -708,7 +735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -727,8 +754,11 @@
       <c r="F2" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="H2" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -747,8 +777,11 @@
       <c r="F3" s="4">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="H3" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -767,8 +800,11 @@
       <c r="F4" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="H4" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -787,8 +823,11 @@
       <c r="F5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="H5" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -807,8 +846,11 @@
       <c r="F6" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="H6" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -827,8 +869,11 @@
       <c r="F7" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="H7" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -847,8 +892,11 @@
       <c r="F8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="H8" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -867,8 +915,11 @@
       <c r="F9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="H9" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
@@ -887,8 +938,11 @@
       <c r="F10" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="H10" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -907,8 +961,11 @@
       <c r="F11" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="H11" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -927,8 +984,11 @@
       <c r="F12" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H12" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>39</v>
       </c>
@@ -947,8 +1007,11 @@
       <c r="F13" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H13" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -967,8 +1030,11 @@
       <c r="F14" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H14" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -987,8 +1053,11 @@
       <c r="F15" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="H15" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
@@ -1007,8 +1076,11 @@
       <c r="F16" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="H16" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>51</v>
       </c>
@@ -1027,8 +1099,11 @@
       <c r="F17" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H17" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>54</v>
       </c>
@@ -1048,7 +1123,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
@@ -1068,7 +1143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>60</v>
       </c>
@@ -1088,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>64</v>
       </c>
@@ -1108,7 +1183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>68</v>
       </c>
@@ -1128,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>71</v>
       </c>
@@ -1148,7 +1223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>74</v>
       </c>
@@ -1168,7 +1243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>77</v>
       </c>
@@ -1188,7 +1263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
Created new Folder for DMB V3.1
</commit_message>
<xml_diff>
--- a/DataManagementBoard_V3/Bill of Materials-DataManagementBoard_V3.xlsx
+++ b/DataManagementBoard_V3/Bill of Materials-DataManagementBoard_V3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\randy\Documents\GitHub\Andromeda-V3.3\DataManagementBoard_V3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2020 - 2021\Andromeda-V3.2\DataManagementBoard_V3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23145B5B-9360-48F9-B0C8-9E0905554FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A06DC4A-E943-491A-9C4A-69C22D781BAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="372" windowWidth="21600" windowHeight="11328" xr2:uid="{3D4BD06D-1139-467C-B010-4B4921899CC2}"/>
+    <workbookView xWindow="-15690" yWindow="2670" windowWidth="14400" windowHeight="7365" xr2:uid="{3D4BD06D-1139-467C-B010-4B4921899CC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-DataManagemen" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="85">
   <si>
     <t>Comment</t>
   </si>
@@ -292,18 +292,6 @@
   </si>
   <si>
     <t>C7, C19</t>
-  </si>
-  <si>
-    <t>BACKORDER</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Backorder</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -333,7 +321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -356,20 +344,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -379,12 +358,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -704,18 +677,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="6" width="18.77734375" customWidth="1"/>
+    <col min="1" max="6" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -735,7 +708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -754,11 +727,8 @@
       <c r="F2" s="4">
         <v>4</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -777,11 +747,8 @@
       <c r="F3" s="4">
         <v>16</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -800,11 +767,8 @@
       <c r="F4" s="4">
         <v>1</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -823,11 +787,8 @@
       <c r="F5" s="4">
         <v>1</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -846,11 +807,8 @@
       <c r="F6" s="4">
         <v>2</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -869,11 +827,8 @@
       <c r="F7" s="4">
         <v>2</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -892,11 +847,8 @@
       <c r="F8" s="4">
         <v>1</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -915,11 +867,8 @@
       <c r="F9" s="4">
         <v>1</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
@@ -938,11 +887,8 @@
       <c r="F10" s="4">
         <v>4</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -961,11 +907,8 @@
       <c r="F11" s="4">
         <v>3</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -984,11 +927,8 @@
       <c r="F12" s="4">
         <v>2</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>39</v>
       </c>
@@ -1007,11 +947,8 @@
       <c r="F13" s="4">
         <v>1</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -1030,11 +967,8 @@
       <c r="F14" s="4">
         <v>3</v>
       </c>
-      <c r="H14" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -1053,11 +987,8 @@
       <c r="F15" s="4">
         <v>2</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
@@ -1076,11 +1007,8 @@
       <c r="F16" s="4">
         <v>1</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>51</v>
       </c>
@@ -1099,11 +1027,8 @@
       <c r="F17" s="4">
         <v>1</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>54</v>
       </c>
@@ -1123,7 +1048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
@@ -1143,7 +1068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>60</v>
       </c>
@@ -1163,7 +1088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>64</v>
       </c>
@@ -1183,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>68</v>
       </c>
@@ -1203,7 +1128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>71</v>
       </c>
@@ -1223,7 +1148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>74</v>
       </c>
@@ -1243,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>77</v>
       </c>
@@ -1263,7 +1188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>81</v>
       </c>

</xml_diff>